<commit_message>
ODA y GOB al 2023
</commit_message>
<xml_diff>
--- a/WB names.xlsx
+++ b/WB names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN_CAP02\Downloads\PortableGit\PES_research-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC4A643A-8832-462C-9966-50BA5F8B3974}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F33AF2-718E-4ADB-A7E3-D335D96FCC1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="7890" xr2:uid="{BCF259E4-46E3-4973-9A7A-CA46AE18EAAC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>NY.GNP.MKTP.KD.ZG</t>
   </si>
@@ -43,6 +43,147 @@
   </si>
   <si>
     <t>Population Growth</t>
+  </si>
+  <si>
+    <t>CC.EST</t>
+  </si>
+  <si>
+    <t>CC.NO.SRC</t>
+  </si>
+  <si>
+    <t>CC.PER.RNK</t>
+  </si>
+  <si>
+    <t>CC.PER.RNK.LOWER</t>
+  </si>
+  <si>
+    <t>CC.PER.RNK.UPPER</t>
+  </si>
+  <si>
+    <t>CC.STD.ERR</t>
+  </si>
+  <si>
+    <t>DT.ODA.ALLD.CD</t>
+  </si>
+  <si>
+    <t>DT.ODA.ALLD.KD</t>
+  </si>
+  <si>
+    <t>DT.ODA.OATL.CD</t>
+  </si>
+  <si>
+    <t>DT.ODA.OATL.KD</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.CD</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.GI.ZS</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.GN.ZS</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.KD</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.MP.ZS</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.PC.ZS</t>
+  </si>
+  <si>
+    <t>DT.ODA.ODAT.XP.ZS</t>
+  </si>
+  <si>
+    <t>GE.EST</t>
+  </si>
+  <si>
+    <t>GE.NO.SRC</t>
+  </si>
+  <si>
+    <t>GE.PER.RNK</t>
+  </si>
+  <si>
+    <t>GE.PER.RNK.LOWER</t>
+  </si>
+  <si>
+    <t>GE.PER.RNK.UPPER</t>
+  </si>
+  <si>
+    <t>GE.STD.ERR</t>
+  </si>
+  <si>
+    <t>PV.EST</t>
+  </si>
+  <si>
+    <t>PV.NO.SRC</t>
+  </si>
+  <si>
+    <t>PV.PER.RNK</t>
+  </si>
+  <si>
+    <t>PV.PER.RNK.LOWER</t>
+  </si>
+  <si>
+    <t>PV.PER.RNK.UPPER</t>
+  </si>
+  <si>
+    <t>PV.STD.ERR</t>
+  </si>
+  <si>
+    <t>RQ.EST</t>
+  </si>
+  <si>
+    <t>RQ.NO.SRC</t>
+  </si>
+  <si>
+    <t>RQ.PER.RNK</t>
+  </si>
+  <si>
+    <t>RQ.PER.RNK.LOWER</t>
+  </si>
+  <si>
+    <t>RQ.PER.RNK.UPPER</t>
+  </si>
+  <si>
+    <t>RQ.STD.ERR</t>
+  </si>
+  <si>
+    <t>RL.ES</t>
+  </si>
+  <si>
+    <t>Net ODA received (% of central government expense)</t>
+  </si>
+  <si>
+    <t>Net ODA received (% of gross capital formation)</t>
+  </si>
+  <si>
+    <t>Net ODA received (% of GNI)</t>
+  </si>
+  <si>
+    <t>Net ODA received (% of imports of goods, services and primary income)</t>
+  </si>
+  <si>
+    <t>Net ODA received per capita (current US$)</t>
+  </si>
+  <si>
+    <t>Net official aid received (constant 2021 US$)</t>
+  </si>
+  <si>
+    <t>Net official aid received (current US$)</t>
+  </si>
+  <si>
+    <t>Net official development assistance and official aid received (constant 2021 US$)</t>
+  </si>
+  <si>
+    <t>Net official development assistance and official aid received (current US$)</t>
+  </si>
+  <si>
+    <t>Net official development assistance received (constant 2021 US$)</t>
+  </si>
+  <si>
+    <t>Net official development assistance received (current US$)</t>
   </si>
 </sst>
 </file>
@@ -78,9 +219,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,15 +537,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEA2083-6E5C-467C-B77C-15A23F81417F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -430,7 +574,222 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Voice and Accountability + models
</commit_message>
<xml_diff>
--- a/WB names.xlsx
+++ b/WB names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN_CAP02\Downloads\PortableGit\PES_research-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F33AF2-718E-4ADB-A7E3-D335D96FCC1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDEAC9F-30D7-43AE-9D96-B519318D6B97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="7890" xr2:uid="{BCF259E4-46E3-4973-9A7A-CA46AE18EAAC}"/>
   </bookViews>
@@ -25,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
-  <si>
-    <t>NY.GNP.MKTP.KD.ZG</t>
-  </si>
-  <si>
-    <t>NY.GNP.PCAP.KD.ZG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>SP.POP.GROW</t>
   </si>
   <si>
-    <t>Gross Net Income Per Capita</t>
-  </si>
-  <si>
-    <t>Gross Net Income</t>
-  </si>
-  <si>
     <t>Population Growth</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t>RQ.STD.ERR</t>
   </si>
   <si>
-    <t>RL.ES</t>
-  </si>
-  <si>
     <t>Net ODA received (% of central government expense)</t>
   </si>
   <si>
@@ -184,6 +169,162 @@
   </si>
   <si>
     <t>Net official development assistance received (current US$)</t>
+  </si>
+  <si>
+    <t>RL.NO.SRC</t>
+  </si>
+  <si>
+    <t>RL.PER.RNK</t>
+  </si>
+  <si>
+    <t>RL.PER.RNK.LOWER</t>
+  </si>
+  <si>
+    <t>RL.PER.RNK.UPPER</t>
+  </si>
+  <si>
+    <t>RL.STD.ERR</t>
+  </si>
+  <si>
+    <t>VA.EST</t>
+  </si>
+  <si>
+    <t>VA.NO.SRC</t>
+  </si>
+  <si>
+    <t>VA.PER.RNK</t>
+  </si>
+  <si>
+    <t>VA.PER.RNK.LOWER</t>
+  </si>
+  <si>
+    <t>VA.PER.RNK.UPPER</t>
+  </si>
+  <si>
+    <t>VA.STD.ERR</t>
+  </si>
+  <si>
+    <t>Rule of Law: Percentile Rank</t>
+  </si>
+  <si>
+    <t>Rule of Law: Percentile Rank, Lower Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Voice and Accountability: Estimate</t>
+  </si>
+  <si>
+    <t>Control of Corruption: Estimate</t>
+  </si>
+  <si>
+    <t>Control of Corruption: Number of sources</t>
+  </si>
+  <si>
+    <t>Control of Corruption: Percentile Rank</t>
+  </si>
+  <si>
+    <t>Control of Corruption: Percentile Rank, Lower Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Control of Corruption: Percentile Rank, Upper Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Control of Corruption: Standard Error</t>
+  </si>
+  <si>
+    <t>Government Effectiveness: Estimate</t>
+  </si>
+  <si>
+    <t>Government Effectiveness: Number of sources</t>
+  </si>
+  <si>
+    <t>Government Effectiveness: Percentile Rank</t>
+  </si>
+  <si>
+    <t>Government Effectiveness: Percentile Rank, Lower Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Government Effectiveness: Percentile Rank, Upper Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Government Effectiveness: Standard Error</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Estimate</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Number of sources</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Percentile Rank</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Percentile Rank, Lower Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Percentile Rank, Upper Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Standard Error</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Estimate</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Number of sources</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Percentile Rank</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Percentile Rank, Lower Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Percentile Rank, Upper Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Standard Error</t>
+  </si>
+  <si>
+    <t>Rule of Law: Estimate</t>
+  </si>
+  <si>
+    <t>Rule of Law: Number of sources</t>
+  </si>
+  <si>
+    <t>Rule of Law: Percentile Rank, Upper Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Rule of Law: Standard Error</t>
+  </si>
+  <si>
+    <t>Voice and Accountability: Number of sources</t>
+  </si>
+  <si>
+    <t>Voice and Accountability: Percentile Rank</t>
+  </si>
+  <si>
+    <t>Voice and Accountability: Percentile Rank, Lower Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Voice and Accountability: Percentile Rank, Upper Bound of 90% Confidence Interval</t>
+  </si>
+  <si>
+    <t>Voice and Accountability: Standard Error</t>
+  </si>
+  <si>
+    <t>NY.GDP.PCAP.CN</t>
+  </si>
+  <si>
+    <t>NY.GDP.PCAP.CD</t>
+  </si>
+  <si>
+    <t>GDP per capita (current LCU)</t>
+  </si>
+  <si>
+    <t>GDP per capita (current US$)</t>
+  </si>
+  <si>
+    <t>RL.EST</t>
   </si>
 </sst>
 </file>
@@ -537,255 +678,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEA2083-6E5C-467C-B77C-15A23F81417F}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>99</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="str">
+        <f>_xlfn.CONCAT("'",SUBSTITUTE(A40,".","_"),"',")</f>
+        <v>'RL_NO_SRC',</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" ref="C41:C50" si="0">_xlfn.CONCAT("'",SUBSTITUTE(A41,".","_"),"',")</f>
+        <v>'RL_PER_RNK',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>'RL_PER_RNK_LOWER',</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>'RL_PER_RNK_UPPER',</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>'RL_STD_ERR',</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>'VA_EST',</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>'VA_NO_SRC',</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>'VA_PER_RNK',</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>'VA_PER_RNK_LOWER',</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>'VA_PER_RNK_UPPER',</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>'VA_STD_ERR',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>